<commit_message>
added from office , view memebr test
</commit_message>
<xml_diff>
--- a/HybridFrameworkApr2019/src/test/resources/Sheets/GAP.xlsx
+++ b/HybridFrameworkApr2019/src/test/resources/Sheets/GAP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="58">
   <si>
     <t>TCID</t>
   </si>
@@ -25,9 +25,6 @@
   </si>
   <si>
     <t>LoginTest</t>
-  </si>
-  <si>
-    <t>TestB</t>
   </si>
   <si>
     <t>TestC</t>
@@ -147,9 +144,6 @@
     <t>Welcome1</t>
   </si>
   <si>
-    <t xml:space="preserve">click </t>
-  </si>
-  <si>
     <t>enrolment_lnk_xpath</t>
   </si>
   <si>
@@ -193,6 +187,9 @@
   </si>
   <si>
     <t>View_MemberTest</t>
+  </si>
+  <si>
+    <t>13900</t>
   </si>
 </sst>
 </file>
@@ -619,7 +616,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,31 +638,31 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -679,7 +676,7 @@
   <dimension ref="A1:AUM19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,19 +694,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:1235" x14ac:dyDescent="0.3">
@@ -718,14 +715,14 @@
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1235" x14ac:dyDescent="0.3">
@@ -734,14 +731,14 @@
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1235" x14ac:dyDescent="0.3">
@@ -750,16 +747,16 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1235" x14ac:dyDescent="0.3">
@@ -768,16 +765,16 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1235" x14ac:dyDescent="0.3">
@@ -786,14 +783,14 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:1235" x14ac:dyDescent="0.3">
@@ -802,23 +799,26 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8"/>
       <c r="H8"/>
@@ -2052,16 +2052,16 @@
     </row>
     <row r="9" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G9"/>
       <c r="H9"/>
@@ -3295,19 +3295,19 @@
     </row>
     <row r="10" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
@@ -4541,19 +4541,19 @@
     </row>
     <row r="11" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
@@ -5787,16 +5787,16 @@
     </row>
     <row r="12" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -7030,13 +7030,13 @@
     </row>
     <row r="13" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G13"/>
       <c r="H13"/>
@@ -8270,16 +8270,16 @@
     </row>
     <row r="14" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G14"/>
       <c r="H14"/>
@@ -9513,16 +9513,16 @@
     </row>
     <row r="15" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
@@ -10756,19 +10756,19 @@
     </row>
     <row r="16" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="F16" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
@@ -12002,19 +12002,19 @@
     </row>
     <row r="17" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G17"/>
       <c r="H17"/>
@@ -13248,19 +13248,19 @@
     </row>
     <row r="18" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G18"/>
       <c r="H18"/>
@@ -14494,19 +14494,19 @@
     </row>
     <row r="19" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G19"/>
       <c r="H19"/>
@@ -15748,13 +15748,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.109375" customWidth="1"/>
     <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
@@ -15770,72 +15770,72 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -15843,73 +15843,73 @@
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>11</v>
+      <c r="F8" s="8" t="s">
+        <v>46</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="G8" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="H8" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
         <v>41</v>
       </c>
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
-      <c r="G9">
-        <v>13900</v>
+      <c r="G9" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -15917,32 +15917,32 @@
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>23</v>
-      </c>
-      <c r="D14" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -15950,35 +15950,36 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated the rediff one from home
</commit_message>
<xml_diff>
--- a/HybridFrameworkApr2019/src/test/resources/Sheets/GAP.xlsx
+++ b/HybridFrameworkApr2019/src/test/resources/Sheets/GAP.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="59">
   <si>
     <t>TCID</t>
   </si>
@@ -191,11 +191,14 @@
   <si>
     <t>13900</t>
   </si>
+  <si>
+    <t>RediffLogin</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -369,7 +372,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -404,7 +407,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -613,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,7 +649,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -663,6 +666,14 @@
       </c>
       <c r="B5" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -673,10 +684,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AUM19"/>
+  <dimension ref="A1:AUM20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15738,6 +15749,11 @@
       <c r="AUL19"/>
       <c r="AUM19"/>
     </row>
+    <row r="20" spans="1:1235" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -15746,10 +15762,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15945,7 +15961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -15956,7 +15972,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -15967,7 +15983,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -15976,6 +15992,30 @@
       </c>
       <c r="C19" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>